<commit_message>
cleaned up folders and finished metadata. added additional analyses for supplement to isotope R script and re-generated figures with productivity axes
</commit_message>
<xml_diff>
--- a/data/isotopes/baseline/2008_Palmyra_Algae Isotopes.xlsx
+++ b/data/isotopes/baseline/2008_Palmyra_Algae Isotopes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuile\Dropbox\2017\Palmyra Isotope Data\Isotopes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/Dropbox/2020/Collaborations/dna_isotopes/data/isotopes/baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9137599-64FF-6043-B8DE-089F618E8B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="11205" xr2:uid="{A58BBF7F-1EA9-4E44-8606-8C379B360485}"/>
+    <workbookView xWindow="0" yWindow="4740" windowWidth="17080" windowHeight="11200" xr2:uid="{A58BBF7F-1EA9-4E44-8606-8C379B360485}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="76">
   <si>
     <t xml:space="preserve">Operator:  </t>
   </si>
@@ -156,12 +157,6 @@
   </si>
   <si>
     <t>C:N</t>
-  </si>
-  <si>
-    <t>KF-N</t>
-  </si>
-  <si>
-    <t>KF-C</t>
   </si>
   <si>
     <t>Run</t>
@@ -765,273 +760,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D84F7C1-B3D6-4D9A-AAA2-CEB93BE99735}">
-  <dimension ref="A1:S63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="M1" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="6.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="4" customWidth="1"/>
-    <col min="257" max="259" width="11.5703125" customWidth="1"/>
-    <col min="260" max="260" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="261" max="269" width="6.85546875" customWidth="1"/>
-    <col min="270" max="270" width="5.5703125" customWidth="1"/>
-    <col min="513" max="515" width="11.5703125" customWidth="1"/>
-    <col min="516" max="516" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="517" max="525" width="6.85546875" customWidth="1"/>
-    <col min="526" max="526" width="5.5703125" customWidth="1"/>
-    <col min="769" max="771" width="11.5703125" customWidth="1"/>
-    <col min="772" max="772" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="773" max="781" width="6.85546875" customWidth="1"/>
-    <col min="782" max="782" width="5.5703125" customWidth="1"/>
-    <col min="1025" max="1027" width="11.5703125" customWidth="1"/>
-    <col min="1028" max="1028" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1037" width="6.85546875" customWidth="1"/>
-    <col min="1038" max="1038" width="5.5703125" customWidth="1"/>
-    <col min="1281" max="1283" width="11.5703125" customWidth="1"/>
-    <col min="1284" max="1284" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1293" width="6.85546875" customWidth="1"/>
-    <col min="1294" max="1294" width="5.5703125" customWidth="1"/>
-    <col min="1537" max="1539" width="11.5703125" customWidth="1"/>
-    <col min="1540" max="1540" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1549" width="6.85546875" customWidth="1"/>
-    <col min="1550" max="1550" width="5.5703125" customWidth="1"/>
-    <col min="1793" max="1795" width="11.5703125" customWidth="1"/>
-    <col min="1796" max="1796" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1805" width="6.85546875" customWidth="1"/>
-    <col min="1806" max="1806" width="5.5703125" customWidth="1"/>
-    <col min="2049" max="2051" width="11.5703125" customWidth="1"/>
-    <col min="2052" max="2052" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2061" width="6.85546875" customWidth="1"/>
-    <col min="2062" max="2062" width="5.5703125" customWidth="1"/>
-    <col min="2305" max="2307" width="11.5703125" customWidth="1"/>
-    <col min="2308" max="2308" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2317" width="6.85546875" customWidth="1"/>
-    <col min="2318" max="2318" width="5.5703125" customWidth="1"/>
-    <col min="2561" max="2563" width="11.5703125" customWidth="1"/>
-    <col min="2564" max="2564" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2573" width="6.85546875" customWidth="1"/>
-    <col min="2574" max="2574" width="5.5703125" customWidth="1"/>
-    <col min="2817" max="2819" width="11.5703125" customWidth="1"/>
-    <col min="2820" max="2820" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2829" width="6.85546875" customWidth="1"/>
-    <col min="2830" max="2830" width="5.5703125" customWidth="1"/>
-    <col min="3073" max="3075" width="11.5703125" customWidth="1"/>
-    <col min="3076" max="3076" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3085" width="6.85546875" customWidth="1"/>
-    <col min="3086" max="3086" width="5.5703125" customWidth="1"/>
-    <col min="3329" max="3331" width="11.5703125" customWidth="1"/>
-    <col min="3332" max="3332" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3341" width="6.85546875" customWidth="1"/>
-    <col min="3342" max="3342" width="5.5703125" customWidth="1"/>
-    <col min="3585" max="3587" width="11.5703125" customWidth="1"/>
-    <col min="3588" max="3588" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3597" width="6.85546875" customWidth="1"/>
-    <col min="3598" max="3598" width="5.5703125" customWidth="1"/>
-    <col min="3841" max="3843" width="11.5703125" customWidth="1"/>
-    <col min="3844" max="3844" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3853" width="6.85546875" customWidth="1"/>
-    <col min="3854" max="3854" width="5.5703125" customWidth="1"/>
-    <col min="4097" max="4099" width="11.5703125" customWidth="1"/>
-    <col min="4100" max="4100" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4109" width="6.85546875" customWidth="1"/>
-    <col min="4110" max="4110" width="5.5703125" customWidth="1"/>
-    <col min="4353" max="4355" width="11.5703125" customWidth="1"/>
-    <col min="4356" max="4356" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4365" width="6.85546875" customWidth="1"/>
-    <col min="4366" max="4366" width="5.5703125" customWidth="1"/>
-    <col min="4609" max="4611" width="11.5703125" customWidth="1"/>
-    <col min="4612" max="4612" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4621" width="6.85546875" customWidth="1"/>
-    <col min="4622" max="4622" width="5.5703125" customWidth="1"/>
-    <col min="4865" max="4867" width="11.5703125" customWidth="1"/>
-    <col min="4868" max="4868" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4877" width="6.85546875" customWidth="1"/>
-    <col min="4878" max="4878" width="5.5703125" customWidth="1"/>
-    <col min="5121" max="5123" width="11.5703125" customWidth="1"/>
-    <col min="5124" max="5124" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5133" width="6.85546875" customWidth="1"/>
-    <col min="5134" max="5134" width="5.5703125" customWidth="1"/>
-    <col min="5377" max="5379" width="11.5703125" customWidth="1"/>
-    <col min="5380" max="5380" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5389" width="6.85546875" customWidth="1"/>
-    <col min="5390" max="5390" width="5.5703125" customWidth="1"/>
-    <col min="5633" max="5635" width="11.5703125" customWidth="1"/>
-    <col min="5636" max="5636" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5645" width="6.85546875" customWidth="1"/>
-    <col min="5646" max="5646" width="5.5703125" customWidth="1"/>
-    <col min="5889" max="5891" width="11.5703125" customWidth="1"/>
-    <col min="5892" max="5892" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5901" width="6.85546875" customWidth="1"/>
-    <col min="5902" max="5902" width="5.5703125" customWidth="1"/>
-    <col min="6145" max="6147" width="11.5703125" customWidth="1"/>
-    <col min="6148" max="6148" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6157" width="6.85546875" customWidth="1"/>
-    <col min="6158" max="6158" width="5.5703125" customWidth="1"/>
-    <col min="6401" max="6403" width="11.5703125" customWidth="1"/>
-    <col min="6404" max="6404" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6413" width="6.85546875" customWidth="1"/>
-    <col min="6414" max="6414" width="5.5703125" customWidth="1"/>
-    <col min="6657" max="6659" width="11.5703125" customWidth="1"/>
-    <col min="6660" max="6660" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6669" width="6.85546875" customWidth="1"/>
-    <col min="6670" max="6670" width="5.5703125" customWidth="1"/>
-    <col min="6913" max="6915" width="11.5703125" customWidth="1"/>
-    <col min="6916" max="6916" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6925" width="6.85546875" customWidth="1"/>
-    <col min="6926" max="6926" width="5.5703125" customWidth="1"/>
-    <col min="7169" max="7171" width="11.5703125" customWidth="1"/>
-    <col min="7172" max="7172" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7181" width="6.85546875" customWidth="1"/>
-    <col min="7182" max="7182" width="5.5703125" customWidth="1"/>
-    <col min="7425" max="7427" width="11.5703125" customWidth="1"/>
-    <col min="7428" max="7428" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7437" width="6.85546875" customWidth="1"/>
-    <col min="7438" max="7438" width="5.5703125" customWidth="1"/>
-    <col min="7681" max="7683" width="11.5703125" customWidth="1"/>
-    <col min="7684" max="7684" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7693" width="6.85546875" customWidth="1"/>
-    <col min="7694" max="7694" width="5.5703125" customWidth="1"/>
-    <col min="7937" max="7939" width="11.5703125" customWidth="1"/>
-    <col min="7940" max="7940" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7949" width="6.85546875" customWidth="1"/>
-    <col min="7950" max="7950" width="5.5703125" customWidth="1"/>
-    <col min="8193" max="8195" width="11.5703125" customWidth="1"/>
-    <col min="8196" max="8196" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8205" width="6.85546875" customWidth="1"/>
-    <col min="8206" max="8206" width="5.5703125" customWidth="1"/>
-    <col min="8449" max="8451" width="11.5703125" customWidth="1"/>
-    <col min="8452" max="8452" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8461" width="6.85546875" customWidth="1"/>
-    <col min="8462" max="8462" width="5.5703125" customWidth="1"/>
-    <col min="8705" max="8707" width="11.5703125" customWidth="1"/>
-    <col min="8708" max="8708" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8717" width="6.85546875" customWidth="1"/>
-    <col min="8718" max="8718" width="5.5703125" customWidth="1"/>
-    <col min="8961" max="8963" width="11.5703125" customWidth="1"/>
-    <col min="8964" max="8964" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8973" width="6.85546875" customWidth="1"/>
-    <col min="8974" max="8974" width="5.5703125" customWidth="1"/>
-    <col min="9217" max="9219" width="11.5703125" customWidth="1"/>
-    <col min="9220" max="9220" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9229" width="6.85546875" customWidth="1"/>
-    <col min="9230" max="9230" width="5.5703125" customWidth="1"/>
-    <col min="9473" max="9475" width="11.5703125" customWidth="1"/>
-    <col min="9476" max="9476" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9485" width="6.85546875" customWidth="1"/>
-    <col min="9486" max="9486" width="5.5703125" customWidth="1"/>
-    <col min="9729" max="9731" width="11.5703125" customWidth="1"/>
-    <col min="9732" max="9732" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9741" width="6.85546875" customWidth="1"/>
-    <col min="9742" max="9742" width="5.5703125" customWidth="1"/>
-    <col min="9985" max="9987" width="11.5703125" customWidth="1"/>
-    <col min="9988" max="9988" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9997" width="6.85546875" customWidth="1"/>
-    <col min="9998" max="9998" width="5.5703125" customWidth="1"/>
-    <col min="10241" max="10243" width="11.5703125" customWidth="1"/>
-    <col min="10244" max="10244" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10253" width="6.85546875" customWidth="1"/>
-    <col min="10254" max="10254" width="5.5703125" customWidth="1"/>
-    <col min="10497" max="10499" width="11.5703125" customWidth="1"/>
-    <col min="10500" max="10500" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10509" width="6.85546875" customWidth="1"/>
-    <col min="10510" max="10510" width="5.5703125" customWidth="1"/>
-    <col min="10753" max="10755" width="11.5703125" customWidth="1"/>
-    <col min="10756" max="10756" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10765" width="6.85546875" customWidth="1"/>
-    <col min="10766" max="10766" width="5.5703125" customWidth="1"/>
-    <col min="11009" max="11011" width="11.5703125" customWidth="1"/>
-    <col min="11012" max="11012" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11021" width="6.85546875" customWidth="1"/>
-    <col min="11022" max="11022" width="5.5703125" customWidth="1"/>
-    <col min="11265" max="11267" width="11.5703125" customWidth="1"/>
-    <col min="11268" max="11268" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11277" width="6.85546875" customWidth="1"/>
-    <col min="11278" max="11278" width="5.5703125" customWidth="1"/>
-    <col min="11521" max="11523" width="11.5703125" customWidth="1"/>
-    <col min="11524" max="11524" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11533" width="6.85546875" customWidth="1"/>
-    <col min="11534" max="11534" width="5.5703125" customWidth="1"/>
-    <col min="11777" max="11779" width="11.5703125" customWidth="1"/>
-    <col min="11780" max="11780" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11789" width="6.85546875" customWidth="1"/>
-    <col min="11790" max="11790" width="5.5703125" customWidth="1"/>
-    <col min="12033" max="12035" width="11.5703125" customWidth="1"/>
-    <col min="12036" max="12036" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12045" width="6.85546875" customWidth="1"/>
-    <col min="12046" max="12046" width="5.5703125" customWidth="1"/>
-    <col min="12289" max="12291" width="11.5703125" customWidth="1"/>
-    <col min="12292" max="12292" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12301" width="6.85546875" customWidth="1"/>
-    <col min="12302" max="12302" width="5.5703125" customWidth="1"/>
-    <col min="12545" max="12547" width="11.5703125" customWidth="1"/>
-    <col min="12548" max="12548" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12557" width="6.85546875" customWidth="1"/>
-    <col min="12558" max="12558" width="5.5703125" customWidth="1"/>
-    <col min="12801" max="12803" width="11.5703125" customWidth="1"/>
-    <col min="12804" max="12804" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12813" width="6.85546875" customWidth="1"/>
-    <col min="12814" max="12814" width="5.5703125" customWidth="1"/>
-    <col min="13057" max="13059" width="11.5703125" customWidth="1"/>
-    <col min="13060" max="13060" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13069" width="6.85546875" customWidth="1"/>
-    <col min="13070" max="13070" width="5.5703125" customWidth="1"/>
-    <col min="13313" max="13315" width="11.5703125" customWidth="1"/>
-    <col min="13316" max="13316" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13325" width="6.85546875" customWidth="1"/>
-    <col min="13326" max="13326" width="5.5703125" customWidth="1"/>
-    <col min="13569" max="13571" width="11.5703125" customWidth="1"/>
-    <col min="13572" max="13572" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13581" width="6.85546875" customWidth="1"/>
-    <col min="13582" max="13582" width="5.5703125" customWidth="1"/>
-    <col min="13825" max="13827" width="11.5703125" customWidth="1"/>
-    <col min="13828" max="13828" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13837" width="6.85546875" customWidth="1"/>
-    <col min="13838" max="13838" width="5.5703125" customWidth="1"/>
-    <col min="14081" max="14083" width="11.5703125" customWidth="1"/>
-    <col min="14084" max="14084" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14093" width="6.85546875" customWidth="1"/>
-    <col min="14094" max="14094" width="5.5703125" customWidth="1"/>
-    <col min="14337" max="14339" width="11.5703125" customWidth="1"/>
-    <col min="14340" max="14340" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14349" width="6.85546875" customWidth="1"/>
-    <col min="14350" max="14350" width="5.5703125" customWidth="1"/>
-    <col min="14593" max="14595" width="11.5703125" customWidth="1"/>
-    <col min="14596" max="14596" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14605" width="6.85546875" customWidth="1"/>
-    <col min="14606" max="14606" width="5.5703125" customWidth="1"/>
-    <col min="14849" max="14851" width="11.5703125" customWidth="1"/>
-    <col min="14852" max="14852" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14861" width="6.85546875" customWidth="1"/>
-    <col min="14862" max="14862" width="5.5703125" customWidth="1"/>
-    <col min="15105" max="15107" width="11.5703125" customWidth="1"/>
-    <col min="15108" max="15108" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15117" width="6.85546875" customWidth="1"/>
-    <col min="15118" max="15118" width="5.5703125" customWidth="1"/>
-    <col min="15361" max="15363" width="11.5703125" customWidth="1"/>
-    <col min="15364" max="15364" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15373" width="6.85546875" customWidth="1"/>
-    <col min="15374" max="15374" width="5.5703125" customWidth="1"/>
-    <col min="15617" max="15619" width="11.5703125" customWidth="1"/>
-    <col min="15620" max="15620" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15629" width="6.85546875" customWidth="1"/>
-    <col min="15630" max="15630" width="5.5703125" customWidth="1"/>
-    <col min="15873" max="15875" width="11.5703125" customWidth="1"/>
-    <col min="15876" max="15876" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15885" width="6.85546875" customWidth="1"/>
-    <col min="15886" max="15886" width="5.5703125" customWidth="1"/>
-    <col min="16129" max="16131" width="11.5703125" customWidth="1"/>
-    <col min="16132" max="16132" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16141" width="6.85546875" customWidth="1"/>
-    <col min="16142" max="16142" width="5.5703125" customWidth="1"/>
+    <col min="1" max="3" width="11.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="6.83203125" style="2" customWidth="1"/>
+    <col min="255" max="257" width="11.5" customWidth="1"/>
+    <col min="258" max="258" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="259" max="267" width="6.83203125" customWidth="1"/>
+    <col min="268" max="268" width="5.5" customWidth="1"/>
+    <col min="511" max="513" width="11.5" customWidth="1"/>
+    <col min="514" max="514" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="515" max="523" width="6.83203125" customWidth="1"/>
+    <col min="524" max="524" width="5.5" customWidth="1"/>
+    <col min="767" max="769" width="11.5" customWidth="1"/>
+    <col min="770" max="770" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="771" max="779" width="6.83203125" customWidth="1"/>
+    <col min="780" max="780" width="5.5" customWidth="1"/>
+    <col min="1023" max="1025" width="11.5" customWidth="1"/>
+    <col min="1026" max="1026" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1035" width="6.83203125" customWidth="1"/>
+    <col min="1036" max="1036" width="5.5" customWidth="1"/>
+    <col min="1279" max="1281" width="11.5" customWidth="1"/>
+    <col min="1282" max="1282" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1291" width="6.83203125" customWidth="1"/>
+    <col min="1292" max="1292" width="5.5" customWidth="1"/>
+    <col min="1535" max="1537" width="11.5" customWidth="1"/>
+    <col min="1538" max="1538" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1547" width="6.83203125" customWidth="1"/>
+    <col min="1548" max="1548" width="5.5" customWidth="1"/>
+    <col min="1791" max="1793" width="11.5" customWidth="1"/>
+    <col min="1794" max="1794" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1803" width="6.83203125" customWidth="1"/>
+    <col min="1804" max="1804" width="5.5" customWidth="1"/>
+    <col min="2047" max="2049" width="11.5" customWidth="1"/>
+    <col min="2050" max="2050" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2059" width="6.83203125" customWidth="1"/>
+    <col min="2060" max="2060" width="5.5" customWidth="1"/>
+    <col min="2303" max="2305" width="11.5" customWidth="1"/>
+    <col min="2306" max="2306" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2315" width="6.83203125" customWidth="1"/>
+    <col min="2316" max="2316" width="5.5" customWidth="1"/>
+    <col min="2559" max="2561" width="11.5" customWidth="1"/>
+    <col min="2562" max="2562" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2571" width="6.83203125" customWidth="1"/>
+    <col min="2572" max="2572" width="5.5" customWidth="1"/>
+    <col min="2815" max="2817" width="11.5" customWidth="1"/>
+    <col min="2818" max="2818" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2827" width="6.83203125" customWidth="1"/>
+    <col min="2828" max="2828" width="5.5" customWidth="1"/>
+    <col min="3071" max="3073" width="11.5" customWidth="1"/>
+    <col min="3074" max="3074" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3083" width="6.83203125" customWidth="1"/>
+    <col min="3084" max="3084" width="5.5" customWidth="1"/>
+    <col min="3327" max="3329" width="11.5" customWidth="1"/>
+    <col min="3330" max="3330" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3339" width="6.83203125" customWidth="1"/>
+    <col min="3340" max="3340" width="5.5" customWidth="1"/>
+    <col min="3583" max="3585" width="11.5" customWidth="1"/>
+    <col min="3586" max="3586" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3595" width="6.83203125" customWidth="1"/>
+    <col min="3596" max="3596" width="5.5" customWidth="1"/>
+    <col min="3839" max="3841" width="11.5" customWidth="1"/>
+    <col min="3842" max="3842" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3851" width="6.83203125" customWidth="1"/>
+    <col min="3852" max="3852" width="5.5" customWidth="1"/>
+    <col min="4095" max="4097" width="11.5" customWidth="1"/>
+    <col min="4098" max="4098" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4107" width="6.83203125" customWidth="1"/>
+    <col min="4108" max="4108" width="5.5" customWidth="1"/>
+    <col min="4351" max="4353" width="11.5" customWidth="1"/>
+    <col min="4354" max="4354" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4363" width="6.83203125" customWidth="1"/>
+    <col min="4364" max="4364" width="5.5" customWidth="1"/>
+    <col min="4607" max="4609" width="11.5" customWidth="1"/>
+    <col min="4610" max="4610" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4619" width="6.83203125" customWidth="1"/>
+    <col min="4620" max="4620" width="5.5" customWidth="1"/>
+    <col min="4863" max="4865" width="11.5" customWidth="1"/>
+    <col min="4866" max="4866" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4875" width="6.83203125" customWidth="1"/>
+    <col min="4876" max="4876" width="5.5" customWidth="1"/>
+    <col min="5119" max="5121" width="11.5" customWidth="1"/>
+    <col min="5122" max="5122" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5131" width="6.83203125" customWidth="1"/>
+    <col min="5132" max="5132" width="5.5" customWidth="1"/>
+    <col min="5375" max="5377" width="11.5" customWidth="1"/>
+    <col min="5378" max="5378" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5387" width="6.83203125" customWidth="1"/>
+    <col min="5388" max="5388" width="5.5" customWidth="1"/>
+    <col min="5631" max="5633" width="11.5" customWidth="1"/>
+    <col min="5634" max="5634" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5643" width="6.83203125" customWidth="1"/>
+    <col min="5644" max="5644" width="5.5" customWidth="1"/>
+    <col min="5887" max="5889" width="11.5" customWidth="1"/>
+    <col min="5890" max="5890" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5899" width="6.83203125" customWidth="1"/>
+    <col min="5900" max="5900" width="5.5" customWidth="1"/>
+    <col min="6143" max="6145" width="11.5" customWidth="1"/>
+    <col min="6146" max="6146" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6155" width="6.83203125" customWidth="1"/>
+    <col min="6156" max="6156" width="5.5" customWidth="1"/>
+    <col min="6399" max="6401" width="11.5" customWidth="1"/>
+    <col min="6402" max="6402" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6411" width="6.83203125" customWidth="1"/>
+    <col min="6412" max="6412" width="5.5" customWidth="1"/>
+    <col min="6655" max="6657" width="11.5" customWidth="1"/>
+    <col min="6658" max="6658" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6667" width="6.83203125" customWidth="1"/>
+    <col min="6668" max="6668" width="5.5" customWidth="1"/>
+    <col min="6911" max="6913" width="11.5" customWidth="1"/>
+    <col min="6914" max="6914" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6923" width="6.83203125" customWidth="1"/>
+    <col min="6924" max="6924" width="5.5" customWidth="1"/>
+    <col min="7167" max="7169" width="11.5" customWidth="1"/>
+    <col min="7170" max="7170" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7179" width="6.83203125" customWidth="1"/>
+    <col min="7180" max="7180" width="5.5" customWidth="1"/>
+    <col min="7423" max="7425" width="11.5" customWidth="1"/>
+    <col min="7426" max="7426" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7435" width="6.83203125" customWidth="1"/>
+    <col min="7436" max="7436" width="5.5" customWidth="1"/>
+    <col min="7679" max="7681" width="11.5" customWidth="1"/>
+    <col min="7682" max="7682" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7691" width="6.83203125" customWidth="1"/>
+    <col min="7692" max="7692" width="5.5" customWidth="1"/>
+    <col min="7935" max="7937" width="11.5" customWidth="1"/>
+    <col min="7938" max="7938" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7947" width="6.83203125" customWidth="1"/>
+    <col min="7948" max="7948" width="5.5" customWidth="1"/>
+    <col min="8191" max="8193" width="11.5" customWidth="1"/>
+    <col min="8194" max="8194" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8203" width="6.83203125" customWidth="1"/>
+    <col min="8204" max="8204" width="5.5" customWidth="1"/>
+    <col min="8447" max="8449" width="11.5" customWidth="1"/>
+    <col min="8450" max="8450" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8459" width="6.83203125" customWidth="1"/>
+    <col min="8460" max="8460" width="5.5" customWidth="1"/>
+    <col min="8703" max="8705" width="11.5" customWidth="1"/>
+    <col min="8706" max="8706" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8715" width="6.83203125" customWidth="1"/>
+    <col min="8716" max="8716" width="5.5" customWidth="1"/>
+    <col min="8959" max="8961" width="11.5" customWidth="1"/>
+    <col min="8962" max="8962" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8971" width="6.83203125" customWidth="1"/>
+    <col min="8972" max="8972" width="5.5" customWidth="1"/>
+    <col min="9215" max="9217" width="11.5" customWidth="1"/>
+    <col min="9218" max="9218" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9227" width="6.83203125" customWidth="1"/>
+    <col min="9228" max="9228" width="5.5" customWidth="1"/>
+    <col min="9471" max="9473" width="11.5" customWidth="1"/>
+    <col min="9474" max="9474" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9483" width="6.83203125" customWidth="1"/>
+    <col min="9484" max="9484" width="5.5" customWidth="1"/>
+    <col min="9727" max="9729" width="11.5" customWidth="1"/>
+    <col min="9730" max="9730" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9739" width="6.83203125" customWidth="1"/>
+    <col min="9740" max="9740" width="5.5" customWidth="1"/>
+    <col min="9983" max="9985" width="11.5" customWidth="1"/>
+    <col min="9986" max="9986" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9995" width="6.83203125" customWidth="1"/>
+    <col min="9996" max="9996" width="5.5" customWidth="1"/>
+    <col min="10239" max="10241" width="11.5" customWidth="1"/>
+    <col min="10242" max="10242" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10251" width="6.83203125" customWidth="1"/>
+    <col min="10252" max="10252" width="5.5" customWidth="1"/>
+    <col min="10495" max="10497" width="11.5" customWidth="1"/>
+    <col min="10498" max="10498" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10507" width="6.83203125" customWidth="1"/>
+    <col min="10508" max="10508" width="5.5" customWidth="1"/>
+    <col min="10751" max="10753" width="11.5" customWidth="1"/>
+    <col min="10754" max="10754" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10763" width="6.83203125" customWidth="1"/>
+    <col min="10764" max="10764" width="5.5" customWidth="1"/>
+    <col min="11007" max="11009" width="11.5" customWidth="1"/>
+    <col min="11010" max="11010" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11019" width="6.83203125" customWidth="1"/>
+    <col min="11020" max="11020" width="5.5" customWidth="1"/>
+    <col min="11263" max="11265" width="11.5" customWidth="1"/>
+    <col min="11266" max="11266" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11275" width="6.83203125" customWidth="1"/>
+    <col min="11276" max="11276" width="5.5" customWidth="1"/>
+    <col min="11519" max="11521" width="11.5" customWidth="1"/>
+    <col min="11522" max="11522" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11531" width="6.83203125" customWidth="1"/>
+    <col min="11532" max="11532" width="5.5" customWidth="1"/>
+    <col min="11775" max="11777" width="11.5" customWidth="1"/>
+    <col min="11778" max="11778" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11787" width="6.83203125" customWidth="1"/>
+    <col min="11788" max="11788" width="5.5" customWidth="1"/>
+    <col min="12031" max="12033" width="11.5" customWidth="1"/>
+    <col min="12034" max="12034" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12043" width="6.83203125" customWidth="1"/>
+    <col min="12044" max="12044" width="5.5" customWidth="1"/>
+    <col min="12287" max="12289" width="11.5" customWidth="1"/>
+    <col min="12290" max="12290" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12299" width="6.83203125" customWidth="1"/>
+    <col min="12300" max="12300" width="5.5" customWidth="1"/>
+    <col min="12543" max="12545" width="11.5" customWidth="1"/>
+    <col min="12546" max="12546" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12555" width="6.83203125" customWidth="1"/>
+    <col min="12556" max="12556" width="5.5" customWidth="1"/>
+    <col min="12799" max="12801" width="11.5" customWidth="1"/>
+    <col min="12802" max="12802" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12811" width="6.83203125" customWidth="1"/>
+    <col min="12812" max="12812" width="5.5" customWidth="1"/>
+    <col min="13055" max="13057" width="11.5" customWidth="1"/>
+    <col min="13058" max="13058" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13067" width="6.83203125" customWidth="1"/>
+    <col min="13068" max="13068" width="5.5" customWidth="1"/>
+    <col min="13311" max="13313" width="11.5" customWidth="1"/>
+    <col min="13314" max="13314" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13323" width="6.83203125" customWidth="1"/>
+    <col min="13324" max="13324" width="5.5" customWidth="1"/>
+    <col min="13567" max="13569" width="11.5" customWidth="1"/>
+    <col min="13570" max="13570" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13579" width="6.83203125" customWidth="1"/>
+    <col min="13580" max="13580" width="5.5" customWidth="1"/>
+    <col min="13823" max="13825" width="11.5" customWidth="1"/>
+    <col min="13826" max="13826" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13835" width="6.83203125" customWidth="1"/>
+    <col min="13836" max="13836" width="5.5" customWidth="1"/>
+    <col min="14079" max="14081" width="11.5" customWidth="1"/>
+    <col min="14082" max="14082" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14091" width="6.83203125" customWidth="1"/>
+    <col min="14092" max="14092" width="5.5" customWidth="1"/>
+    <col min="14335" max="14337" width="11.5" customWidth="1"/>
+    <col min="14338" max="14338" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14347" width="6.83203125" customWidth="1"/>
+    <col min="14348" max="14348" width="5.5" customWidth="1"/>
+    <col min="14591" max="14593" width="11.5" customWidth="1"/>
+    <col min="14594" max="14594" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14603" width="6.83203125" customWidth="1"/>
+    <col min="14604" max="14604" width="5.5" customWidth="1"/>
+    <col min="14847" max="14849" width="11.5" customWidth="1"/>
+    <col min="14850" max="14850" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14859" width="6.83203125" customWidth="1"/>
+    <col min="14860" max="14860" width="5.5" customWidth="1"/>
+    <col min="15103" max="15105" width="11.5" customWidth="1"/>
+    <col min="15106" max="15106" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15115" width="6.83203125" customWidth="1"/>
+    <col min="15116" max="15116" width="5.5" customWidth="1"/>
+    <col min="15359" max="15361" width="11.5" customWidth="1"/>
+    <col min="15362" max="15362" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15371" width="6.83203125" customWidth="1"/>
+    <col min="15372" max="15372" width="5.5" customWidth="1"/>
+    <col min="15615" max="15617" width="11.5" customWidth="1"/>
+    <col min="15618" max="15618" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15627" width="6.83203125" customWidth="1"/>
+    <col min="15628" max="15628" width="5.5" customWidth="1"/>
+    <col min="15871" max="15873" width="11.5" customWidth="1"/>
+    <col min="15874" max="15874" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15883" width="6.83203125" customWidth="1"/>
+    <col min="15884" max="15884" width="5.5" customWidth="1"/>
+    <col min="16127" max="16129" width="11.5" customWidth="1"/>
+    <col min="16130" max="16130" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16139" width="6.83203125" customWidth="1"/>
+    <col min="16140" max="16140" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1059,7 +1053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1073,12 +1067,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1115,44 +1109,36 @@
       <c r="L5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>39939</v>
       </c>
@@ -1163,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="11">
         <v>4.96</v>
@@ -1189,12 +1175,11 @@
       <c r="L7" s="12">
         <v>21.079676948693436</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="4">
+      <c r="M7" s="4">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>39939</v>
       </c>
@@ -1205,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="11">
         <v>4.7729999999999997</v>
@@ -1231,12 +1216,11 @@
       <c r="L8" s="12">
         <v>19.097694172523841</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="4">
+      <c r="M8" s="4">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>39939</v>
       </c>
@@ -1247,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="11">
         <v>4.79</v>
@@ -1273,12 +1257,11 @@
       <c r="L9" s="12">
         <v>16.300150171880944</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="4">
+      <c r="M9" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>39939</v>
       </c>
@@ -1289,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11">
         <v>5.0039999999999996</v>
@@ -1315,12 +1298,11 @@
       <c r="L10" s="12">
         <v>43.321993228609948</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="4">
+      <c r="M10" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>39939</v>
       </c>
@@ -1331,7 +1313,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="11">
         <v>4.8730000000000002</v>
@@ -1357,12 +1339,11 @@
       <c r="L11" s="12">
         <v>28.178831459771018</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="4">
+      <c r="M11" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>39939</v>
       </c>
@@ -1373,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>4.827</v>
@@ -1399,12 +1380,11 @@
       <c r="L12" s="12">
         <v>44.221880737964298</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="4">
+      <c r="M12" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>39939</v>
       </c>
@@ -1415,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11">
         <v>5.0140000000000002</v>
@@ -1441,12 +1421,11 @@
       <c r="L13" s="12">
         <v>36.159789727045549</v>
       </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="4">
+      <c r="M13" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>39939</v>
       </c>
@@ -1457,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" s="11">
         <v>4.7350000000000003</v>
@@ -1483,12 +1462,11 @@
       <c r="L14" s="12">
         <v>66.09224319735921</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="4">
+      <c r="M14" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>39939</v>
       </c>
@@ -1499,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="11">
         <v>4.915</v>
@@ -1525,12 +1503,11 @@
       <c r="L15" s="12">
         <v>60.55025978961325</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="4">
+      <c r="M15" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>39939</v>
       </c>
@@ -1541,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16" s="11">
         <v>5.1029999999999998</v>
@@ -1567,12 +1544,11 @@
       <c r="L16" s="12">
         <v>3.2439960372091599</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="4">
+      <c r="M16" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>39939</v>
       </c>
@@ -1583,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="11">
         <v>4.62</v>
@@ -1609,12 +1585,11 @@
       <c r="L17" s="12">
         <v>27.729109714628972</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="4">
+      <c r="M17" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>39939</v>
       </c>
@@ -1625,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" s="11">
         <v>4.8029999999999999</v>
@@ -1651,12 +1626,11 @@
       <c r="L18" s="12">
         <v>3.2439960372091603</v>
       </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="4">
+      <c r="M18" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>39939</v>
       </c>
@@ -1667,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" s="11">
         <v>4.7050000000000001</v>
@@ -1693,12 +1667,11 @@
       <c r="L19" s="12">
         <v>31.29444011559919</v>
       </c>
-      <c r="N19" s="2"/>
-      <c r="O19" s="4">
+      <c r="M19" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>39939</v>
       </c>
@@ -1709,7 +1682,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E20" s="11">
         <v>5.0759999999999996</v>
@@ -1735,12 +1708,11 @@
       <c r="L20" s="12">
         <v>64.880077048125457</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="4">
+      <c r="M20" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>39939</v>
       </c>
@@ -1751,7 +1723,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" s="11">
         <v>5.04</v>
@@ -1777,12 +1749,11 @@
       <c r="L21" s="12">
         <v>46.274530256493776</v>
       </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="4">
+      <c r="M21" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>39939</v>
       </c>
@@ -1793,7 +1764,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" s="11">
         <v>4.6879999999999997</v>
@@ -1819,12 +1790,11 @@
       <c r="L22" s="12">
         <v>24.77036515297609</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="4">
+      <c r="M22" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>39939</v>
       </c>
@@ -1835,7 +1805,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E23" s="11">
         <v>4.7</v>
@@ -1861,12 +1831,11 @@
       <c r="L23" s="12">
         <v>19.879498890846779</v>
       </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="4">
+      <c r="M23" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>39939</v>
       </c>
@@ -1877,7 +1846,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" s="11">
         <v>4.9740000000000002</v>
@@ -1903,12 +1872,11 @@
       <c r="L24" s="12">
         <v>20.730653678022037</v>
       </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="4">
+      <c r="M24" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>39939</v>
       </c>
@@ -1919,7 +1887,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" s="11">
         <v>4.7089999999999996</v>
@@ -1945,12 +1913,11 @@
       <c r="L25" s="12">
         <v>32.933533219232146</v>
       </c>
-      <c r="N25" s="2"/>
-      <c r="O25" s="4">
+      <c r="M25" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>39939</v>
       </c>
@@ -1961,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E26" s="11">
         <v>5.1439999999999992</v>
@@ -1987,12 +1954,11 @@
       <c r="L26" s="12">
         <v>61.594242956378345</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="4">
+      <c r="M26" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>39939</v>
       </c>
@@ -2003,7 +1969,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E27" s="11">
         <v>4.84</v>
@@ -2029,12 +1995,11 @@
       <c r="L27" s="12">
         <v>55.636131185117229</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="4">
+      <c r="M27" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>39939</v>
       </c>
@@ -2045,7 +2010,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E28" s="11">
         <v>4.7679999999999998</v>
@@ -2071,12 +2036,11 @@
       <c r="L28" s="12">
         <v>40.335281945295414</v>
       </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="4">
+      <c r="M28" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>39939</v>
       </c>
@@ -2087,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E29" s="11">
         <v>4.7629999999999999</v>
@@ -2113,12 +2077,11 @@
       <c r="L29" s="12">
         <v>66.752466397630556</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="4">
+      <c r="M29" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>39939</v>
       </c>
@@ -2129,7 +2092,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E30" s="11">
         <v>4.8380000000000001</v>
@@ -2155,23 +2118,22 @@
       <c r="L30" s="12">
         <v>64.056166839510468</v>
       </c>
-      <c r="N30" s="2"/>
-      <c r="O30" s="4">
+      <c r="M30" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>39993</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="E31" s="11">
         <v>3.5859999999999994</v>
@@ -2197,27 +2159,26 @@
       <c r="L31" s="12">
         <v>29.683879498728501</v>
       </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="4">
+      <c r="M31" s="4">
         <v>9</v>
       </c>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="4"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N31" s="12"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>39993</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E32" s="11">
         <v>3.6360000000000006</v>
@@ -2243,27 +2204,26 @@
       <c r="L32" s="12">
         <v>22.843718266222339</v>
       </c>
+      <c r="M32" s="4">
+        <v>10</v>
+      </c>
       <c r="N32" s="2"/>
-      <c r="O32" s="4">
-        <v>10</v>
-      </c>
+      <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="4"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q32" s="4"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>39993</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E33" s="11">
         <v>3.504</v>
@@ -2289,27 +2249,26 @@
       <c r="L33" s="12">
         <v>25.553451998877687</v>
       </c>
+      <c r="M33" s="4">
+        <v>11</v>
+      </c>
       <c r="N33" s="2"/>
-      <c r="O33" s="4">
-        <v>11</v>
-      </c>
+      <c r="O33" s="2"/>
       <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="4"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>39993</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E34" s="11">
         <v>3.625</v>
@@ -2335,23 +2294,22 @@
       <c r="L34" s="12">
         <v>23.528726803951653</v>
       </c>
-      <c r="N34" s="2"/>
-      <c r="O34" s="4">
+      <c r="M34" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>39993</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E35" s="11">
         <v>3.4350000000000001</v>
@@ -2377,23 +2335,22 @@
       <c r="L35" s="12">
         <v>22.375579338013647</v>
       </c>
-      <c r="N35" s="2"/>
-      <c r="O35" s="4">
+      <c r="M35" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>39993</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E36" s="11">
         <v>3.609</v>
@@ -2419,23 +2376,22 @@
       <c r="L36" s="12">
         <v>39.411708390309663</v>
       </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="4">
+      <c r="M36" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>39993</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E37" s="11">
         <v>3.4580000000000002</v>
@@ -2461,23 +2417,22 @@
       <c r="L37" s="12">
         <v>33.833045983679305</v>
       </c>
-      <c r="N37" s="2"/>
-      <c r="O37" s="4">
+      <c r="M37" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>39993</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="11">
         <v>3.4870000000000001</v>
@@ -2503,23 +2458,22 @@
       <c r="L38" s="12">
         <v>25.499203673583395</v>
       </c>
-      <c r="N38" s="2"/>
-      <c r="O38" s="4">
+      <c r="M38" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>39993</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E39" s="11">
         <v>3.419</v>
@@ -2545,23 +2499,22 @@
       <c r="L39" s="12">
         <v>27.183715279531018</v>
       </c>
-      <c r="N39" s="2"/>
-      <c r="O39" s="4">
+      <c r="M39" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <v>39993</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E40" s="11">
         <v>3.4430000000000001</v>
@@ -2587,23 +2540,22 @@
       <c r="L40" s="12">
         <v>24.791653678092445</v>
       </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="4">
+      <c r="M40" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>39993</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E41" s="11">
         <v>3.4929999999999999</v>
@@ -2629,23 +2581,22 @@
       <c r="L41" s="12">
         <v>19.569787945747475</v>
       </c>
-      <c r="N41" s="2"/>
-      <c r="O41" s="4">
+      <c r="M41" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>39993</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E42" s="11">
         <v>3.5129999999999999</v>
@@ -2671,23 +2622,22 @@
       <c r="L42" s="12">
         <v>21.130674084702893</v>
       </c>
-      <c r="N42" s="2"/>
-      <c r="O42" s="4">
+      <c r="M42" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>39993</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E43" s="11">
         <v>3.488</v>
@@ -2713,23 +2663,22 @@
       <c r="L43" s="12">
         <v>21.465372486157982</v>
       </c>
-      <c r="N43" s="2"/>
-      <c r="O43" s="4">
+      <c r="M43" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>39993</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E44" s="11">
         <v>3.48</v>
@@ -2755,23 +2704,22 @@
       <c r="L44" s="12">
         <v>19.362456310853823</v>
       </c>
-      <c r="N44" s="2"/>
-      <c r="O44" s="4">
+      <c r="M44" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>39993</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E45" s="11">
         <v>3.5609999999999995</v>
@@ -2797,23 +2745,22 @@
       <c r="L45" s="12">
         <v>20.516981641446989</v>
       </c>
-      <c r="N45" s="2"/>
-      <c r="O45" s="4">
+      <c r="M45" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>39993</v>
       </c>
       <c r="B46" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="E46" s="11">
         <v>2.9689999999999999</v>
@@ -2839,23 +2786,22 @@
       <c r="L46" s="12">
         <v>17.488089601356076</v>
       </c>
-      <c r="N46" s="2"/>
-      <c r="O46" s="4">
+      <c r="M46" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>39993</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E47" s="11">
         <v>3.0139999999999998</v>
@@ -2881,23 +2827,22 @@
       <c r="L47" s="12">
         <v>14.638581374185986</v>
       </c>
-      <c r="N47" s="2"/>
-      <c r="O47" s="4">
+      <c r="M47" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>39993</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E48" s="11">
         <v>2.9020000000000001</v>
@@ -2923,23 +2868,22 @@
       <c r="L48" s="12">
         <v>17.460872130437934</v>
       </c>
-      <c r="N48" s="2"/>
-      <c r="O48" s="4">
+      <c r="M48" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>39993</v>
       </c>
       <c r="B49" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="E49" s="11">
         <v>3.0979999999999994</v>
@@ -2965,23 +2909,22 @@
       <c r="L49" s="12">
         <v>20.891626449783566</v>
       </c>
-      <c r="N49" s="2"/>
-      <c r="O49" s="4">
+      <c r="M49" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>39993</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E50" s="11">
         <v>3</v>
@@ -3007,23 +2950,22 @@
       <c r="L50" s="12">
         <v>18.991741334618268</v>
       </c>
-      <c r="N50" s="2"/>
-      <c r="O50" s="4">
+      <c r="M50" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>39993</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E51" s="11">
         <v>2.9060000000000001</v>
@@ -3049,23 +2991,22 @@
       <c r="L51" s="12">
         <v>20.768881158372025</v>
       </c>
-      <c r="N51" s="2"/>
-      <c r="O51" s="4">
+      <c r="M51" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>39993</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E52" s="11">
         <v>2.9470000000000001</v>
@@ -3091,23 +3032,22 @@
       <c r="L52" s="12">
         <v>20.474290524355386</v>
       </c>
-      <c r="N52" s="2"/>
-      <c r="O52" s="4">
+      <c r="M52" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>39993</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E53" s="11">
         <v>3.0470000000000002</v>
@@ -3133,23 +3073,22 @@
       <c r="L53" s="12">
         <v>21.81670426904293</v>
       </c>
-      <c r="N53" s="2"/>
-      <c r="O53" s="4">
+      <c r="M53" s="4">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>39993</v>
       </c>
       <c r="B54" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="E54" s="11">
         <v>8.5190000000000001</v>
@@ -3175,23 +3114,22 @@
       <c r="L54" s="12">
         <v>39.946938545194328</v>
       </c>
-      <c r="N54" s="2"/>
-      <c r="O54" s="4">
+      <c r="M54" s="4">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>39993</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E55" s="11">
         <v>2.5919999999999996</v>
@@ -3217,23 +3155,22 @@
       <c r="L55" s="12">
         <v>14.960473277484958</v>
       </c>
-      <c r="N55" s="2"/>
-      <c r="O55" s="4">
+      <c r="M55" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>39993</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E56" s="11">
         <v>8.4909999999999997</v>
@@ -3259,23 +3196,22 @@
       <c r="L56" s="12">
         <v>18.902643945354473</v>
       </c>
-      <c r="N56" s="2"/>
-      <c r="O56" s="4">
+      <c r="M56" s="4">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>39993</v>
       </c>
       <c r="B57" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="E57" s="11">
         <v>0.95499999999999996</v>
@@ -3301,23 +3237,22 @@
       <c r="L57" s="12">
         <v>4.7574277289148839</v>
       </c>
-      <c r="N57" s="2"/>
-      <c r="O57" s="4">
+      <c r="M57" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>39993</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E58" s="11">
         <v>0.91800000000000004</v>
@@ -3343,23 +3278,22 @@
       <c r="L58" s="12">
         <v>11.689362375226546</v>
       </c>
-      <c r="N58" s="2"/>
-      <c r="O58" s="4">
+      <c r="M58" s="4">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>39993</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E59" s="11">
         <v>0.96599999999999997</v>
@@ -3385,23 +3319,22 @@
       <c r="L59" s="12">
         <v>19.457248547920067</v>
       </c>
-      <c r="N59" s="2"/>
-      <c r="O59" s="4">
+      <c r="M59" s="4">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>39993</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E60" s="11">
         <v>0.95899999999999996</v>
@@ -3427,23 +3360,22 @@
       <c r="L60" s="12">
         <v>5.1695472801231119</v>
       </c>
-      <c r="N60" s="2"/>
-      <c r="O60" s="4">
+      <c r="M60" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>39993</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E61" s="11">
         <v>0.86399999999999999</v>
@@ -3469,23 +3401,22 @@
       <c r="L61" s="12">
         <v>10.668039105103794</v>
       </c>
-      <c r="N61" s="2"/>
-      <c r="O61" s="4">
+      <c r="M61" s="4">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>39993</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E62" s="11">
         <v>0.86399999999999999</v>
@@ -3511,23 +3442,22 @@
       <c r="L62" s="12">
         <v>20.598460874060795</v>
       </c>
-      <c r="N62" s="2"/>
-      <c r="O62" s="4">
+      <c r="M62" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>39993</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E63" s="11">
         <v>0.878</v>
@@ -3553,8 +3483,7 @@
       <c r="L63" s="12">
         <v>18.705178507988858</v>
       </c>
-      <c r="N63" s="2"/>
-      <c r="O63" s="4">
+      <c r="M63" s="4">
         <v>46</v>
       </c>
     </row>

</xml_diff>